<commit_message>
Updated BOM with correct items Added LED Controller.c to easily control which LED is on.
</commit_message>
<xml_diff>
--- a/Hardware/BOM/LED_Watch_BOM.xlsx
+++ b/Hardware/BOM/LED_Watch_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>Part</t>
   </si>
@@ -139,13 +139,22 @@
   </si>
   <si>
     <t>PM indictor LED</t>
+  </si>
+  <si>
+    <t>445-8919-1-ND</t>
+  </si>
+  <si>
+    <t>10 uF decoupling</t>
+  </si>
+  <si>
+    <t>490-6125-1-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +176,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -185,15 +202,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,7 +516,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,6 +609,12 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -658,6 +684,17 @@
         <v>25</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
@@ -707,8 +744,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" display="http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=178538991&amp;uq=635760440624849824"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Improved crystal board layout, added reverse voltage protection with schottky diode. Fixed incorrect capacitor package sizes.
</commit_message>
<xml_diff>
--- a/Hardware/BOM/LED_Watch_BOM.xlsx
+++ b/Hardware/BOM/LED_Watch_BOM.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Harrington\Documents\Electronic Projects\LED_Watch\Hardware\BOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="18585" windowHeight="7125"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>Part</t>
   </si>
@@ -148,12 +153,39 @@
   </si>
   <si>
     <t>490-6125-1-ND</t>
+  </si>
+  <si>
+    <t>Compatibility for v1.1</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>JTI</t>
+  </si>
+  <si>
+    <t>712-1220-1-ND</t>
+  </si>
+  <si>
+    <t>Checked in v1.1</t>
+  </si>
+  <si>
+    <t>Size correct - Check crystal specs</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>0402 2.2 nF Decoupling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,12 +217,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -206,11 +244,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -221,6 +260,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -269,7 +311,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -302,9 +344,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -337,6 +396,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -513,20 +589,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="85.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="5" max="5" width="37" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,22 +620,32 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -570,8 +658,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -588,7 +679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -605,7 +696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -616,7 +707,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -632,8 +723,11 @@
       <c r="E7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -649,8 +743,11 @@
       <c r="E8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -666,8 +763,11 @@
       <c r="E9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -683,8 +783,14 @@
       <c r="E10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -694,8 +800,11 @@
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -708,8 +817,11 @@
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -725,8 +837,11 @@
       <c r="E13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -741,6 +856,49 @@
       </c>
       <c r="E14" t="s">
         <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expanded board size slightly to ensure switch contacts do not touch LED contacts. Added more silkscreen, fixed size of PM LED
</commit_message>
<xml_diff>
--- a/Hardware/BOM/LED_Watch_BOM.xlsx
+++ b/Hardware/BOM/LED_Watch_BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>Part</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>Checked in v1.1</t>
-  </si>
-  <si>
-    <t>Size correct - Check crystal specs</t>
   </si>
   <si>
     <t>?</t>
@@ -592,7 +589,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +881,7 @@
         <v>45</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -892,13 +889,13 @@
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>